<commit_message>
modified structure of cm individual table and removed localStorage
</commit_message>
<xml_diff>
--- a/assets/excel/Production_Data_Modified.xlsx
+++ b/assets/excel/Production_Data_Modified.xlsx
@@ -455,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -474,6 +474,9 @@
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="10" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="2" fillId="0" fontId="3" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -4051,7 +4054,7 @@
       <c r="F12" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="16" t="s">
         <v>76</v>
       </c>
       <c r="H12" s="11" t="s">
@@ -4092,49 +4095,49 @@
       <c r="C13" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="17">
         <v>0.3006</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="17">
         <v>0.306612</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="17">
         <v>0.31274424</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="17">
         <v>0.31899912480000003</v>
       </c>
-      <c r="H13" s="17">
-        <v>0.315379107296</v>
-      </c>
-      <c r="I13" s="16">
+      <c r="H13" s="18">
+        <v>0.345379107296</v>
+      </c>
+      <c r="I13" s="17">
         <v>0.33188668944192007</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="17">
         <v>0.3385244232307585</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="18">
         <v>0.355294911695374</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="17">
         <v>0.35220080992928116</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="17">
         <v>0.3592448261278668</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="17">
         <v>0.3664297226504241</v>
       </c>
-      <c r="O13" s="16">
+      <c r="O13" s="17">
         <v>0.3737583171034326</v>
       </c>
-      <c r="P13" s="16">
+      <c r="P13" s="17">
         <v>0.3812334834455013</v>
       </c>
-      <c r="Q13" s="16">
+      <c r="Q13" s="17">
         <v>0.3888581531144113</v>
       </c>
-      <c r="R13" s="16">
+      <c r="R13" s="17">
         <v>0.3966353161766995</v>
       </c>
     </row>
@@ -4189,7 +4192,7 @@
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -6727,61 +6730,61 @@
       <c r="C8" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="20">
         <v>0.02</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="20">
         <f t="shared" ref="E8:M8" si="2">D8*1.02</f>
         <v>0.0204</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="20">
         <f t="shared" si="2"/>
         <v>0.020808</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="20">
         <f t="shared" si="2"/>
         <v>0.02122416</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="20">
         <f t="shared" si="2"/>
         <v>0.0216486432</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="20">
         <f t="shared" si="2"/>
         <v>0.02208161606</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="20">
         <f t="shared" si="2"/>
         <v>0.02252324839</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="20">
         <f t="shared" si="2"/>
         <v>0.02297371335</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="20">
         <f t="shared" si="2"/>
         <v>0.02343318762</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="20">
         <f t="shared" si="2"/>
         <v>0.02390185137</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="20">
         <v>0.03</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="20">
         <f t="shared" ref="O8:R8" si="3">N8*1.02</f>
         <v>0.0306</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="20">
         <f t="shared" si="3"/>
         <v>0.031212</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="Q8" s="20">
         <f t="shared" si="3"/>
         <v>0.03183624</v>
       </c>
-      <c r="R8" s="19">
+      <c r="R8" s="20">
         <f t="shared" si="3"/>
         <v>0.0324729648</v>
       </c>
@@ -6790,49 +6793,49 @@
       <c r="C9" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="21">
         <v>56.0</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="21">
         <v>57.120000000000005</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="21">
         <v>58.26240000000001</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="21">
         <v>59.427648000000005</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="21">
         <v>60.61620096000001</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="21">
         <v>61.82852497920001</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="21">
         <v>63.065095478784016</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="21">
         <v>64.3263973883597</v>
       </c>
-      <c r="L9" s="20">
+      <c r="L9" s="21">
         <v>65.61292533612689</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="21">
         <v>66.92518384284944</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="22">
         <v>68.26368751970642</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="22">
         <v>69.62896127010055</v>
       </c>
-      <c r="P9" s="21">
+      <c r="P9" s="22">
         <v>71.02154049550256</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="22">
         <v>72.44197130541262</v>
       </c>
-      <c r="R9" s="21">
+      <c r="R9" s="22">
         <v>73.89081073152087</v>
       </c>
     </row>
@@ -6846,7 +6849,7 @@
       <c r="E10" s="15">
         <v>4337.7846</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="23">
         <v>4424.540292</v>
       </c>
       <c r="G10" s="15">
@@ -6896,7 +6899,7 @@
       <c r="E11" s="11">
         <v>35.0</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="16">
         <v>35.0</v>
       </c>
       <c r="G11" s="11">
@@ -7020,10 +7023,10 @@
       <c r="M13" s="15">
         <v>1736.14682721469</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="23">
         <v>1770.86976375898</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="23">
         <v>1806.28715903416</v>
       </c>
       <c r="P13" s="15">
@@ -8055,7 +8058,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="D1" s="23">
+      <c r="D1" s="24">
         <v>45597.0</v>
       </c>
       <c r="R1" s="5"/>
@@ -8281,7 +8284,7 @@
       <c r="J6" s="15">
         <v>128.713740037056</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="25">
         <v>0.0</v>
       </c>
       <c r="L6" s="15">
@@ -8296,7 +8299,7 @@
       <c r="O6" s="15">
         <v>142.11036948298883</v>
       </c>
-      <c r="P6" s="25">
+      <c r="P6" s="26">
         <v>0.0</v>
       </c>
       <c r="Q6" s="15">
@@ -8331,7 +8334,7 @@
       <c r="J7" s="15">
         <v>0.0</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="25">
         <f t="shared" ref="K7:K8" si="1">MIN(5%*K5,7)</f>
         <v>6.564400742</v>
       </c>
@@ -8347,14 +8350,14 @@
       <c r="O7" s="15">
         <v>0.0</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="27">
         <f>5%*P5</f>
         <v>7.247628844</v>
       </c>
       <c r="Q7" s="15">
         <v>0.0</v>
       </c>
-      <c r="R7" s="26">
+      <c r="R7" s="27">
         <f>5%*R5</f>
         <v>7.540433049</v>
       </c>
@@ -8372,7 +8375,7 @@
       <c r="F8" s="15">
         <v>0.0</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="27" t="s">
         <v>94</v>
       </c>
       <c r="H8" s="15">
@@ -8388,7 +8391,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="24" t="s">
+      <c r="L8" s="25" t="s">
         <v>95</v>
       </c>
       <c r="M8" s="15">

</xml_diff>